<commit_message>
add MS et def pour start et end c0cf33744968fed81748caf22df95daa3b6711d9
</commit_message>
<xml_diff>
--- a/sd-MS-availabletime-healthcareservice/ig/StructureDefinition-ror-healthcareservice.xlsx
+++ b/sd-MS-availabletime-healthcareservice/ig/StructureDefinition-ror-healthcareservice.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-09T10:53:49+00:00</t>
+    <t>2024-02-09T11:04:15+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1933,7 +1933,7 @@
 </t>
   </si>
   <si>
-    <t>Opening time of day (ignored if allDay = true)</t>
+    <t>heureDebut (Horaire) : Heure de début de la plage horaire</t>
   </si>
   <si>
     <t>The opening time of day. Note: If the AllDay flag is set, then this time is ignored.</t>
@@ -1945,7 +1945,7 @@
     <t>HealthcareService.availableTime.availableEndTime</t>
   </si>
   <si>
-    <t>Closing time of day (ignored if allDay = true)</t>
+    <t>heureFin (Horaire) : Heure de fin de la plage horaire</t>
   </si>
   <si>
     <t>The closing time of day. Note: If the AllDay flag is set, then this time is ignored.</t>
@@ -19440,7 +19440,7 @@
         <v>83</v>
       </c>
       <c r="H158" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I158" t="s" s="2">
         <v>74</v>
@@ -19548,7 +19548,7 @@
         <v>83</v>
       </c>
       <c r="H159" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I159" t="s" s="2">
         <v>74</v>

</xml_diff>